<commit_message>
Updating code with new data
</commit_message>
<xml_diff>
--- a/FwaEu.MediCare/DevelopmentData/Users/ApplicationUsers.xlsx
+++ b/FwaEu.MediCare/DevelopmentData/Users/ApplicationUsers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MediCare\CODE\FwaEu.MediCare\DevelopmentData\Users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D10702A-8A58-436C-AA28-9BB51463D889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34379192-9F1A-48E3-B7E0-F1557314289A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="22290" windowHeight="13305" xr2:uid="{43C42DAA-9BC9-4F54-BD14-49579A69BE36}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Data type:</t>
   </si>
@@ -87,12 +87,6 @@
   </si>
   <si>
     <t>BOUTAIB</t>
-  </si>
-  <si>
-    <t>IsAdmin</t>
-  </si>
-  <si>
-    <t>Est administrateur</t>
   </si>
   <si>
     <t>FwaEu.MediCare.Users.Import.ApplicationUserImportModel, FwaEu.MediCare</t>
@@ -564,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBEADCD-88C2-40D8-BF50-20C6D385BA0C}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,10 +570,9 @@
     <col min="2" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -587,19 +580,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>3</v>
       </c>
@@ -608,9 +601,8 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>4</v>
       </c>
@@ -629,11 +621,8 @@
       <c r="F12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>5</v>
@@ -650,11 +639,8 @@
       <c r="F13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="11" t="s">
         <v>15</v>
@@ -669,31 +655,25 @@
         <v>8</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="10" t="b">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="10" t="b">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update database config + add services for patients and buildings
</commit_message>
<xml_diff>
--- a/FwaEu.MediCare/DevelopmentData/Users/ApplicationUsers.xlsx
+++ b/FwaEu.MediCare/DevelopmentData/Users/ApplicationUsers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MediCare\CODE\FwaEu.MediCare\DevelopmentData\Users\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MediaCare\FwaEu.MediCare\DevelopmentData\Users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34379192-9F1A-48E3-B7E0-F1557314289A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF060D9-C762-45DF-BD69-F994BA6B9CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22290" windowHeight="13305" xr2:uid="{43C42DAA-9BC9-4F54-BD14-49579A69BE36}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{43C42DAA-9BC9-4F54-BD14-49579A69BE36}"/>
   </bookViews>
   <sheets>
     <sheet name="Utilisateurs" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Data type:</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>dimitri@fwa.eu</t>
+  </si>
+  <si>
+    <t>Dimitri</t>
+  </si>
+  <si>
+    <t>ASHIKHMIN</t>
   </si>
 </sst>
 </file>
@@ -558,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBEADCD-88C2-40D8-BF50-20C6D385BA0C}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,10 +685,29 @@
         <v>22</v>
       </c>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B14" r:id="rId1" xr:uid="{1D3BA4A9-20DC-446F-9167-80C9ECAC3E15}"/>
     <hyperlink ref="B15" r:id="rId2" xr:uid="{33018842-E2F3-42DB-ADA4-B22285DA937E}"/>
+    <hyperlink ref="B16" r:id="rId3" xr:uid="{93706AA9-1FCC-43E5-8508-D5513C887059}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Login property to Application user
</commit_message>
<xml_diff>
--- a/FwaEu.MediCare/DevelopmentData/Users/ApplicationUsers.xlsx
+++ b/FwaEu.MediCare/DevelopmentData/Users/ApplicationUsers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MediaCare\FwaEu.MediCare\DevelopmentData\Users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF060D9-C762-45DF-BD69-F994BA6B9CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FD1A93-956A-46A9-A700-F8ED79A3CC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{43C42DAA-9BC9-4F54-BD14-49579A69BE36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{43C42DAA-9BC9-4F54-BD14-49579A69BE36}"/>
   </bookViews>
   <sheets>
     <sheet name="Utilisateurs" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Data type:</t>
   </si>
@@ -111,6 +111,18 @@
   </si>
   <si>
     <t>ASHIKHMIN</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>soufian</t>
+  </si>
+  <si>
+    <t>mathis</t>
+  </si>
+  <si>
+    <t>dimitri</t>
   </si>
 </sst>
 </file>
@@ -567,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBEADCD-88C2-40D8-BF50-20C6D385BA0C}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +593,7 @@
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -589,7 +601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -601,7 +613,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>3</v>
       </c>
@@ -610,8 +622,9 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>4</v>
       </c>
@@ -630,8 +643,11 @@
       <c r="F12" s="8" t="s">
         <v>9</v>
       </c>
+      <c r="G12" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>5</v>
@@ -648,8 +664,11 @@
       <c r="F13" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="G13" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="11" t="s">
         <v>15</v>
@@ -666,8 +685,11 @@
       <c r="F14" s="10" t="s">
         <v>22</v>
       </c>
+      <c r="G14" s="10" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="12" t="s">
         <v>19</v>
@@ -684,8 +706,11 @@
       <c r="F15" s="10" t="s">
         <v>22</v>
       </c>
+      <c r="G15" s="10" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="12" t="s">
         <v>23</v>
@@ -701,6 +726,9 @@
       </c>
       <c r="F16" s="10" t="s">
         <v>22</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update backgroundtask and adding create or update handler
</commit_message>
<xml_diff>
--- a/FwaEu.MediCare/DevelopmentData/Users/ApplicationUsers.xlsx
+++ b/FwaEu.MediCare/DevelopmentData/Users/ApplicationUsers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MediaCare\FwaEu.MediCare\DevelopmentData\Users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FD1A93-956A-46A9-A700-F8ED79A3CC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8293369A-6076-427E-8180-AC1213893B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{43C42DAA-9BC9-4F54-BD14-49579A69BE36}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Data type:</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>dimitri</t>
+  </si>
+  <si>
+    <t>support@fwa.eu</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>ROBOT</t>
+  </si>
+  <si>
+    <t>supportrobot</t>
   </si>
 </sst>
 </file>
@@ -579,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBEADCD-88C2-40D8-BF50-20C6D385BA0C}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,13 +683,13 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="11" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>8</v>
@@ -686,7 +698,7 @@
         <v>22</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -729,6 +741,27 @@
       </c>
       <c r="G16" s="10" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -736,6 +769,7 @@
     <hyperlink ref="B14" r:id="rId1" xr:uid="{1D3BA4A9-20DC-446F-9167-80C9ECAC3E15}"/>
     <hyperlink ref="B15" r:id="rId2" xr:uid="{33018842-E2F3-42DB-ADA4-B22285DA937E}"/>
     <hyperlink ref="B16" r:id="rId3" xr:uid="{93706AA9-1FCC-43E5-8508-D5513C887059}"/>
+    <hyperlink ref="B17" r:id="rId4" xr:uid="{561BAACB-6786-43F8-9C25-EF90DDF38255}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>